<commit_message>
añadido filtro fechas//memoria avanzada
Entramos en el endgame
</commit_message>
<xml_diff>
--- a/codigo/antenas.xlsx
+++ b/codigo/antenas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t xml:space="preserve">MCC</t>
   </si>
@@ -287,7 +287,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -453,8 +453,8 @@
       <c r="D6" s="4" t="n">
         <v>3013</v>
       </c>
-      <c r="E6" s="5" t="n">
-        <v>701866</v>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>17</v>

</xml_diff>